<commit_message>
Update retirement process estimates
</commit_message>
<xml_diff>
--- a/input/reg_home_ownership.xlsx
+++ b/input/reg_home_ownership.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPathsFork\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F838EC-AEC2-47EC-99A1-843B20AF8BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8EE0ED-53BF-4FCD-89B2-3E55E06E2BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21480" windowHeight="12675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
-    <sheet name="HO1a" sheetId="5" r:id="rId2"/>
+    <sheet name="HU_HO1a" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>